<commit_message>
finalizado DDL e DML
</commit_message>
<xml_diff>
--- a/Modelagem/modelagem-spmedicalgroup-fisico.xlsx
+++ b/Modelagem/modelagem-spmedicalgroup-fisico.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20354"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39221000826\Documents\senai_spmedgroup_sprint1_bd_manha_flavio_pires\Modelagem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fdnpi\OneDrive\Área de Trabalho\Senai\Projetos Senai\senai_spmedgroup_sprint1_bd_manha_flavio_pires\Modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EE7B30-4CC4-41B3-8707-E610C030C993}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{37EE7B30-4CC4-41B3-8707-E610C030C993}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB9B0029-4E25-4A17-8D74-F253F2E5C3F8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{4D6D4549-E603-4A5D-9E44-FB70F3D58B9C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4D6D4549-E603-4A5D-9E44-FB70F3D58B9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -87,9 +87,6 @@
     <t>IdUsuario</t>
   </si>
   <si>
-    <t>Nome</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -388,13 +385,16 @@
   </si>
   <si>
     <t>TituloSituacao</t>
+  </si>
+  <si>
+    <t>NomeUsuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,27 +423,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF4A4A4A"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
@@ -615,7 +594,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -639,9 +618,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -653,10 +629,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="3" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1023,32 +996,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78804989-D715-43AA-A111-C435CB443992}">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="66.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="66.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1068,7 +1041,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -1088,17 +1061,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="D6" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="41"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="35"/>
+      <c r="D6" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="37"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1106,13 +1079,13 @@
         <v>14</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>1</v>
       </c>
@@ -1123,10 +1096,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>2</v>
       </c>
@@ -1137,10 +1110,10 @@
         <v>2</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>3</v>
       </c>
@@ -1151,174 +1124,174 @@
         <v>3</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" s="10">
         <v>4</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="10">
         <v>5</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="10">
         <v>6</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="10">
         <v>7</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="B15" s="37"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="33"/>
       <c r="D15" s="10">
         <v>8</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="32" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="28" t="s">
         <v>119</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>120</v>
       </c>
       <c r="D16" s="10">
         <v>9</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="33">
-        <v>1</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>111</v>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="29">
+        <v>1</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>110</v>
       </c>
       <c r="D17" s="10">
         <v>10</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="33">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="29">
         <v>2</v>
       </c>
-      <c r="B18" s="34" t="s">
-        <v>113</v>
+      <c r="B18" s="30" t="s">
+        <v>112</v>
       </c>
       <c r="D18" s="10">
         <v>11</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="33">
-        <v>3</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>112</v>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="29">
+        <v>3</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>111</v>
       </c>
       <c r="D19" s="10">
         <v>12</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D20" s="10">
         <v>13</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D21" s="10">
         <v>14</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D22" s="10">
         <v>15</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D23" s="10">
         <v>16</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D24" s="10">
         <v>17</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H24" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="40" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>19</v>
       </c>
@@ -1329,16 +1302,16 @@
         <v>1</v>
       </c>
       <c r="D28" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>1</v>
       </c>
@@ -1352,13 +1325,13 @@
         <v>15</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>2</v>
       </c>
@@ -1369,16 +1342,16 @@
         <v>1</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>3</v>
       </c>
@@ -1389,16 +1362,16 @@
         <v>1</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>4</v>
       </c>
@@ -1409,16 +1382,16 @@
         <v>1</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>5</v>
       </c>
@@ -1428,17 +1401,17 @@
       <c r="C33" s="12">
         <v>1</v>
       </c>
-      <c r="D33" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>41</v>
+      <c r="D33" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>6</v>
       </c>
@@ -1448,17 +1421,17 @@
       <c r="C34" s="12">
         <v>1</v>
       </c>
-      <c r="D34" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>42</v>
+      <c r="D34" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>7</v>
       </c>
@@ -1468,17 +1441,17 @@
       <c r="C35" s="12">
         <v>1</v>
       </c>
-      <c r="D35" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>43</v>
+      <c r="D35" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>8</v>
       </c>
@@ -1488,17 +1461,17 @@
       <c r="C36" s="12">
         <v>1</v>
       </c>
-      <c r="D36" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>44</v>
+      <c r="D36" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>9</v>
       </c>
@@ -1508,17 +1481,17 @@
       <c r="C37" s="12">
         <v>1</v>
       </c>
-      <c r="D37" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>45</v>
+      <c r="D37" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>10</v>
       </c>
@@ -1528,17 +1501,17 @@
       <c r="C38" s="12">
         <v>1</v>
       </c>
-      <c r="D38" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>46</v>
+      <c r="D38" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>11</v>
       </c>
@@ -1548,436 +1521,436 @@
       <c r="C39" s="12">
         <v>1</v>
       </c>
-      <c r="D39" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>47</v>
+      <c r="D39" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="18" t="s">
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="18" t="s">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="16">
+        <v>1</v>
+      </c>
+      <c r="B44" s="16">
+        <v>2</v>
+      </c>
+      <c r="C44" s="16">
+        <v>2</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="16">
+        <v>2</v>
+      </c>
+      <c r="B45" s="16">
+        <v>3</v>
+      </c>
+      <c r="C45" s="16">
+        <v>17</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="16">
+        <v>3</v>
+      </c>
+      <c r="B46" s="16">
+        <v>4</v>
+      </c>
+      <c r="C46" s="16">
+        <v>16</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="39"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D43" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="19">
-        <v>1</v>
-      </c>
-      <c r="B44" s="19">
+      <c r="C50" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G50" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="19">
+        <v>1</v>
+      </c>
+      <c r="B51" s="19">
+        <v>5</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" s="20">
+        <v>94839859000</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F51" s="21">
+        <v>30602</v>
+      </c>
+      <c r="G51" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="19">
         <v>2</v>
       </c>
-      <c r="C44" s="19">
+      <c r="B52" s="19">
+        <v>6</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" s="20">
+        <v>73556944057</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F52" s="21">
+        <v>37095</v>
+      </c>
+      <c r="G52" s="22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="19">
+        <v>3</v>
+      </c>
+      <c r="B53" s="19">
+        <v>7</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53" s="20">
+        <v>16839338002</v>
+      </c>
+      <c r="E53" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F53" s="21">
+        <v>28773</v>
+      </c>
+      <c r="G53" s="22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="19">
+        <v>4</v>
+      </c>
+      <c r="B54" s="19">
+        <v>8</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D54" s="20">
+        <v>14332654765</v>
+      </c>
+      <c r="E54" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="F54" s="21">
+        <v>31333</v>
+      </c>
+      <c r="G54" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="19">
+        <v>5</v>
+      </c>
+      <c r="B55" s="19">
+        <v>9</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D55" s="20">
+        <v>91305348010</v>
+      </c>
+      <c r="E55" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F55" s="21">
+        <v>27633</v>
+      </c>
+      <c r="G55" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="19">
+        <v>6</v>
+      </c>
+      <c r="B56" s="19">
+        <v>10</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D56" s="20">
+        <v>79799299004</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F56" s="21">
+        <v>26379</v>
+      </c>
+      <c r="G56" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="19">
+        <v>7</v>
+      </c>
+      <c r="B57" s="19">
+        <v>11</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D57" s="20">
+        <v>13771913039</v>
+      </c>
+      <c r="E57" s="23"/>
+      <c r="F57" s="21">
+        <v>43164</v>
+      </c>
+      <c r="G57" s="22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="B60" s="32"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D61" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="25">
+        <v>1</v>
+      </c>
+      <c r="B62" s="25">
+        <v>3</v>
+      </c>
+      <c r="C62" s="25">
+        <v>7</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="E62" s="27">
+        <v>43850.625</v>
+      </c>
+      <c r="F62" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="25">
         <v>2</v>
       </c>
-      <c r="D44" s="20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="19">
+      <c r="B63" s="25">
         <v>2</v>
       </c>
-      <c r="B45" s="19">
-        <v>3</v>
-      </c>
-      <c r="C45" s="19">
-        <v>17</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="19">
-        <v>3</v>
-      </c>
-      <c r="B46" s="19">
+      <c r="C63" s="25">
+        <v>2</v>
+      </c>
+      <c r="D63" s="26"/>
+      <c r="E63" s="27">
+        <v>43836.416666666664</v>
+      </c>
+      <c r="F63" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="25">
+        <v>3</v>
+      </c>
+      <c r="B64" s="25">
+        <v>2</v>
+      </c>
+      <c r="C64" s="25">
+        <v>3</v>
+      </c>
+      <c r="D64" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="E64" s="27">
+        <v>43868.458333333336</v>
+      </c>
+      <c r="F64" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="25">
         <v>4</v>
       </c>
-      <c r="C46" s="19">
-        <v>16</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="B49" s="43"/>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="43"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B50" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C50" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D50" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E50" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F50" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="G50" s="21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="22">
-        <v>1</v>
-      </c>
-      <c r="B51" s="22">
+      <c r="B65" s="25">
+        <v>2</v>
+      </c>
+      <c r="C65" s="25">
+        <v>2</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="E65" s="27">
+        <v>43137.416666666664</v>
+      </c>
+      <c r="F65" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="25">
         <v>5</v>
       </c>
-      <c r="C51" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="D51" s="23">
-        <v>94839859000</v>
-      </c>
-      <c r="E51" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="F51" s="24">
-        <v>30602</v>
-      </c>
-      <c r="G51" s="25" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="22">
+      <c r="B66" s="25">
+        <v>1</v>
+      </c>
+      <c r="C66" s="25">
+        <v>4</v>
+      </c>
+      <c r="D66" s="26"/>
+      <c r="E66" s="27">
+        <v>43503.458854166667</v>
+      </c>
+      <c r="F66" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="25">
+        <v>6</v>
+      </c>
+      <c r="B67" s="25">
+        <v>3</v>
+      </c>
+      <c r="C67" s="25">
+        <v>7</v>
+      </c>
+      <c r="D67" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="E67" s="27">
+        <v>43898.625</v>
+      </c>
+      <c r="F67" s="31">
         <v>2</v>
       </c>
-      <c r="B52" s="22">
-        <v>6</v>
-      </c>
-      <c r="C52" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D52" s="23">
-        <v>73556944057</v>
-      </c>
-      <c r="E52" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="F52" s="24">
-        <v>37095</v>
-      </c>
-      <c r="G52" s="26" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="22">
-        <v>3</v>
-      </c>
-      <c r="B53" s="22">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="25">
         <v>7</v>
       </c>
-      <c r="C53" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="D53" s="23">
-        <v>16839338002</v>
-      </c>
-      <c r="E53" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="F53" s="24">
-        <v>28773</v>
-      </c>
-      <c r="G53" s="26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="22">
+      <c r="B68" s="25">
+        <v>1</v>
+      </c>
+      <c r="C68" s="25">
         <v>4</v>
       </c>
-      <c r="B54" s="22">
-        <v>8</v>
-      </c>
-      <c r="C54" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="D54" s="23">
-        <v>14332654765</v>
-      </c>
-      <c r="E54" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="F54" s="24">
-        <v>31333</v>
-      </c>
-      <c r="G54" s="26" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="22">
-        <v>5</v>
-      </c>
-      <c r="B55" s="22">
-        <v>9</v>
-      </c>
-      <c r="C55" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="D55" s="23">
-        <v>91305348010</v>
-      </c>
-      <c r="E55" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="F55" s="24">
-        <v>27633</v>
-      </c>
-      <c r="G55" s="26" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="22">
-        <v>6</v>
-      </c>
-      <c r="B56" s="22">
-        <v>10</v>
-      </c>
-      <c r="C56" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="D56" s="23">
-        <v>79799299004</v>
-      </c>
-      <c r="E56" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="F56" s="24">
-        <v>26379</v>
-      </c>
-      <c r="G56" s="26" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="22">
-        <v>7</v>
-      </c>
-      <c r="B57" s="22">
-        <v>11</v>
-      </c>
-      <c r="C57" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D57" s="23">
-        <v>13771913039</v>
-      </c>
-      <c r="E57" s="27"/>
-      <c r="F57" s="24">
-        <v>43164</v>
-      </c>
-      <c r="G57" s="26" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
-      <c r="F60" s="36"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="B61" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C61" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="D61" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="E61" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="F61" s="28" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="29">
-        <v>1</v>
-      </c>
-      <c r="B62" s="29">
-        <v>3</v>
-      </c>
-      <c r="C62" s="29">
-        <v>7</v>
-      </c>
-      <c r="D62" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="E62" s="31">
-        <v>43850.625</v>
-      </c>
-      <c r="F62" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="29">
-        <v>2</v>
-      </c>
-      <c r="B63" s="29">
-        <v>2</v>
-      </c>
-      <c r="C63" s="29">
-        <v>2</v>
-      </c>
-      <c r="D63" s="30"/>
-      <c r="E63" s="31">
-        <v>43836.416666666664</v>
-      </c>
-      <c r="F63" s="35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="29">
-        <v>3</v>
-      </c>
-      <c r="B64" s="29">
-        <v>2</v>
-      </c>
-      <c r="C64" s="29">
-        <v>3</v>
-      </c>
-      <c r="D64" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="E64" s="31">
-        <v>43868.458333333336</v>
-      </c>
-      <c r="F64" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="29">
-        <v>4</v>
-      </c>
-      <c r="B65" s="29">
-        <v>2</v>
-      </c>
-      <c r="C65" s="29">
-        <v>2</v>
-      </c>
-      <c r="D65" s="30" t="s">
+      <c r="D68" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="E65" s="31">
-        <v>43137.416666666664</v>
-      </c>
-      <c r="F65" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="29">
-        <v>5</v>
-      </c>
-      <c r="B66" s="29">
-        <v>1</v>
-      </c>
-      <c r="C66" s="29">
-        <v>4</v>
-      </c>
-      <c r="D66" s="30"/>
-      <c r="E66" s="31">
-        <v>43503.458854166667</v>
-      </c>
-      <c r="F66" s="35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="29">
-        <v>6</v>
-      </c>
-      <c r="B67" s="29">
-        <v>3</v>
-      </c>
-      <c r="C67" s="29">
-        <v>7</v>
-      </c>
-      <c r="D67" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="E67" s="31">
-        <v>43898.625</v>
-      </c>
-      <c r="F67" s="35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="29">
-        <v>7</v>
-      </c>
-      <c r="B68" s="29">
-        <v>1</v>
-      </c>
-      <c r="C68" s="29">
-        <v>4</v>
-      </c>
-      <c r="D68" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="E68" s="31">
+      <c r="E68" s="27">
         <v>43899.458854166667</v>
       </c>
-      <c r="F68" s="35">
+      <c r="F68" s="31">
         <v>2</v>
       </c>
     </row>

</xml_diff>